<commit_message>
Security Fix: Removed Leaked Credentials & Added .gitignore
</commit_message>
<xml_diff>
--- a/Paper Trading Simulator/paper_trade_book.xlsx
+++ b/Paper Trading Simulator/paper_trade_book.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Shivendra -PC Sync\Google AntiGravity\Paper Trading Simulator\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE65BA1A-E685-49B9-AE39-69562D1EC25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="TradeBook" sheetId="1" r:id="rId1"/>
@@ -18,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TradeBook!$A$1:$R$25</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="49">
   <si>
     <t>Buy Date</t>
   </si>
@@ -77,6 +71,15 @@
   </si>
   <si>
     <t>PnL_Percentage</t>
+  </si>
+  <si>
+    <t>12/29/2025</t>
+  </si>
+  <si>
+    <t>12/30/2025</t>
+  </si>
+  <si>
+    <t>2025-12-31</t>
   </si>
   <si>
     <t>ADANIENT</t>
@@ -166,8 +169,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,33 +228,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -289,7 +283,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -323,7 +317,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -358,10 +351,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -534,35 +526,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="8" width="18.6640625" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" customWidth="1"/>
-    <col min="18" max="18" width="16.6640625" customWidth="1"/>
+    <col min="1" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,24 +610,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>46020</v>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>2203.1999999999998</v>
+        <v>2203.2</v>
       </c>
       <c r="G2">
         <v>4</v>
@@ -644,10 +636,10 @@
         <v>4</v>
       </c>
       <c r="I2">
-        <v>8812.7999999999993</v>
+        <v>8812.799999999999</v>
       </c>
       <c r="J2">
-        <v>2239.6999999999998</v>
+        <v>2239.7</v>
       </c>
       <c r="L2">
         <v>2093.04</v>
@@ -668,18 +660,18 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>46020</v>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -697,10 +689,10 @@
         <v>9856</v>
       </c>
       <c r="J3">
-        <v>1269.4000000000001</v>
+        <v>1269.4</v>
       </c>
       <c r="L3">
-        <v>1170.4000000000001</v>
+        <v>1170.4</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -718,18 +710,18 @@
         <v>3.04</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>46020</v>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -768,18 +760,18 @@
         <v>-0.17</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>46020</v>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -794,7 +786,7 @@
         <v>3</v>
       </c>
       <c r="I5">
-        <v>8527.2000000000007</v>
+        <v>8527.200000000001</v>
       </c>
       <c r="J5">
         <v>2829</v>
@@ -809,33 +801,33 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>-40.200000000000003</v>
+        <v>-40.2</v>
       </c>
       <c r="Q5">
-        <v>-40.200000000000003</v>
+        <v>-40.2</v>
       </c>
       <c r="R5">
         <v>-0.47</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>46020</v>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>2293.3000000000002</v>
+        <v>2293.3</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -844,7 +836,7 @@
         <v>4</v>
       </c>
       <c r="I6">
-        <v>9173.2000000000007</v>
+        <v>9173.200000000001</v>
       </c>
       <c r="J6">
         <v>2315.9</v>
@@ -859,27 +851,27 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>90.4</v>
+        <v>90.40000000000001</v>
       </c>
       <c r="Q6">
-        <v>90.4</v>
+        <v>90.40000000000001</v>
       </c>
       <c r="R6">
         <v>0.99</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>46020</v>
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -918,18 +910,18 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>46020</v>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -968,18 +960,18 @@
         <v>-0.08</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>46020</v>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1015,21 +1007,21 @@
         <v>27</v>
       </c>
       <c r="R9">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>46020</v>
+        <v>0.29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" t="s">
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1044,7 +1036,7 @@
         <v>3</v>
       </c>
       <c r="I10">
-        <v>9227.7000000000007</v>
+        <v>9227.700000000001</v>
       </c>
       <c r="J10">
         <v>3075</v>
@@ -1068,18 +1060,18 @@
         <v>-0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>46020</v>
+    <row r="11" spans="1:18">
+      <c r="A11" t="s">
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1115,21 +1107,21 @@
         <v>451.24</v>
       </c>
       <c r="R11">
-        <v>4.5199999999999996</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>46020</v>
+        <v>4.52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" t="s">
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1168,18 +1160,18 @@
         <v>-1.33</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>46020</v>
+    <row r="13" spans="1:18">
+      <c r="A13" t="s">
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1209,33 +1201,33 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <v>290.39999999999998</v>
+        <v>290.4</v>
       </c>
       <c r="Q13">
-        <v>290.39999999999998</v>
+        <v>290.4</v>
       </c>
       <c r="R13">
         <v>3.14</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>46020</v>
+    <row r="14" spans="1:18">
+      <c r="A14" t="s">
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>651.20000000000005</v>
+        <v>651.2</v>
       </c>
       <c r="G14">
         <v>15</v>
@@ -1268,18 +1260,18 @@
         <v>2.62</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>46020</v>
+    <row r="15" spans="1:18">
+      <c r="A15" t="s">
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1318,18 +1310,18 @@
         <v>-0.27</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>46020</v>
+    <row r="16" spans="1:18">
+      <c r="A16" t="s">
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1368,18 +1360,18 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>46021</v>
+    <row r="17" spans="1:18">
+      <c r="A17" t="s">
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1418,18 +1410,18 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>46021</v>
+    <row r="18" spans="1:18">
+      <c r="A18" t="s">
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1450,7 +1442,7 @@
         <v>287.45</v>
       </c>
       <c r="L18">
-        <v>268.66000000000003</v>
+        <v>268.66</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -1468,18 +1460,18 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>46021</v>
+    <row r="19" spans="1:18">
+      <c r="A19" t="s">
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1518,18 +1510,18 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>46021</v>
+    <row r="20" spans="1:18">
+      <c r="A20" t="s">
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1568,18 +1560,18 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>46021</v>
+    <row r="21" spans="1:18">
+      <c r="A21" t="s">
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1594,7 +1586,7 @@
         <v>81</v>
       </c>
       <c r="I21">
-        <v>9912.7800000000007</v>
+        <v>9912.780000000001</v>
       </c>
       <c r="J21">
         <v>123.58</v>
@@ -1618,18 +1610,18 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>46021</v>
+    <row r="22" spans="1:18">
+      <c r="A22" t="s">
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1659,33 +1651,33 @@
         <v>0</v>
       </c>
       <c r="P22">
-        <v>154.80000000000001</v>
+        <v>154.8</v>
       </c>
       <c r="Q22">
-        <v>154.80000000000001</v>
+        <v>154.8</v>
       </c>
       <c r="R22">
         <v>1.95</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>46021</v>
+    <row r="23" spans="1:18">
+      <c r="A23" t="s">
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>1024.1500000000001</v>
+        <v>1024.15</v>
       </c>
       <c r="G23">
         <v>9</v>
@@ -1697,10 +1689,10 @@
         <v>9217.35</v>
       </c>
       <c r="J23">
-        <v>1027.3499999999999</v>
+        <v>1027.35</v>
       </c>
       <c r="L23">
-        <v>972.94</v>
+        <v>972.9400000000001</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -1718,18 +1710,18 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>46022</v>
+    <row r="24" spans="1:18">
+      <c r="A24" t="s">
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1750,7 +1742,7 @@
         <v>166.46</v>
       </c>
       <c r="L24">
-        <v>158.13999999999999</v>
+        <v>158.14</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -1768,18 +1760,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>46022</v>
+    <row r="25" spans="1:18">
+      <c r="A25" t="s">
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1794,7 +1786,7 @@
         <v>9</v>
       </c>
       <c r="I25">
-        <v>9484.2000000000007</v>
+        <v>9484.200000000001</v>
       </c>
       <c r="J25">
         <v>1053.8</v>
@@ -1819,8 +1811,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R25" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:R25"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>